<commit_message>
Right before moving all span-related information to the 'Evaluation' tab and file
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Feasibility Criteria" sheetId="3" r:id="rId2"/>
     <sheet name="Decision Points" sheetId="4" r:id="rId3"/>
+    <sheet name="Per linear m costs" sheetId="5" r:id="rId4"/>
+    <sheet name="Lumpsum costs" sheetId="6" r:id="rId5"/>
+    <sheet name="Default Unit Costs" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$H$25</definedName>
@@ -64,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="179">
   <si>
     <t>Construction method</t>
   </si>
@@ -541,6 +544,66 @@
   </si>
   <si>
     <t xml:space="preserve">Streambed slope &gt; 2%? </t>
+  </si>
+  <si>
+    <t>Steel Decking</t>
+  </si>
+  <si>
+    <t>Crossbeams + Bolts</t>
+  </si>
+  <si>
+    <t>Fencing System</t>
+  </si>
+  <si>
+    <t>Restraint and Handrail Wires</t>
+  </si>
+  <si>
+    <t>Cables and Clips</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Per linear m cost (RWF)</t>
+  </si>
+  <si>
+    <t>Per linear m cost (USD)</t>
+  </si>
+  <si>
+    <t>Steel Reinforcement</t>
+  </si>
+  <si>
+    <t>Concrete Works</t>
+  </si>
+  <si>
+    <t>Lumpsum cost (RWF)</t>
+  </si>
+  <si>
+    <t>Lumpsum cost (USD)</t>
+  </si>
+  <si>
+    <t>Cement Cost/50kg bag (USD)</t>
+  </si>
+  <si>
+    <t>Steel Cost/kg (USD)</t>
+  </si>
+  <si>
+    <t>Skilled Labor Cost/man-day (USD)</t>
+  </si>
+  <si>
+    <t>Masonry Cost/m3 (USD)</t>
+  </si>
+  <si>
+    <t>Sand Cost/m3 (USD)</t>
+  </si>
+  <si>
+    <t>Aggregate (20mm) Cost/m3 (USD)</t>
+  </si>
+  <si>
+    <t>Unskilled Labor Cost/man-day (USD)</t>
+  </si>
+  <si>
+    <t>Unit cost</t>
   </si>
 </sst>
 </file>
@@ -815,7 +878,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -872,10 +935,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1818,10 +1883,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="36"/>
+      <c r="B2" s="37"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1895,10 +1960,10 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="36"/>
+      <c r="B15" s="37"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1945,10 +2010,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="36"/>
+      <c r="B25" s="37"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -2004,7 +2069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -2131,7 +2196,7 @@
       <c r="C5" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="36">
         <v>0.02</v>
       </c>
       <c r="E5" t="s">
@@ -2151,4 +2216,231 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2">
+        <v>115000</v>
+      </c>
+      <c r="C2">
+        <f>B2*0.00089</f>
+        <v>102.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3">
+        <v>70000</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C6" si="0">B3*0.00089</f>
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4">
+        <v>15000</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>13.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5">
+        <v>15000</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>13.35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6">
+        <v>250000</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>222.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="38">
+        <v>10700000</v>
+      </c>
+      <c r="C2">
+        <f>B2*0.00089</f>
+        <v>9523</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="38">
+        <v>820000</v>
+      </c>
+      <c r="C3">
+        <f>B3*0.00089</f>
+        <v>729.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working live version 14_08_23
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -9,18 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Feasibility Criteria" sheetId="3" r:id="rId2"/>
-    <sheet name="Decision Points" sheetId="4" r:id="rId3"/>
-    <sheet name="Per linear m costs" sheetId="5" r:id="rId4"/>
-    <sheet name="Lumpsum costs" sheetId="6" r:id="rId5"/>
-    <sheet name="Default Unit Costs" sheetId="7" r:id="rId6"/>
+    <sheet name="Decision Points_orig" sheetId="8" r:id="rId3"/>
+    <sheet name="Decision Points" sheetId="4" r:id="rId4"/>
+    <sheet name="Per linear m costs_suspension" sheetId="10" r:id="rId5"/>
+    <sheet name="Per linear m costs_suspended" sheetId="5" r:id="rId6"/>
+    <sheet name="Lumpsum costs_suspension" sheetId="9" r:id="rId7"/>
+    <sheet name="Lumpsum costs_suspended" sheetId="6" r:id="rId8"/>
+    <sheet name="Default Unit Costs" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$H$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$I$25</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +40,7 @@
     <author>Mwendwa KIKO</author>
   </authors>
   <commentList>
-    <comment ref="G16" authorId="0" shapeId="0">
+    <comment ref="H16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="198">
   <si>
     <t>Construction method</t>
   </si>
@@ -93,9 +96,6 @@
     <t>Suspended Cable Bridge</t>
   </si>
   <si>
-    <t>Timber Log Footbridges</t>
-  </si>
-  <si>
     <t>Box Culvert</t>
   </si>
   <si>
@@ -186,9 +186,6 @@
     <t>Mandays for skilled labour: 1.3 x span + 400; Mandays for unskilled labour: 5 x span + 400</t>
   </si>
   <si>
-    <t>Ontario Ministry of Transport Guide|http://www.bv.transports.gouv.qc.ca/mono/1165314.pdf; Florida DOT manual|https://fdotwww.blob.core.windows.net/sitefinity/docs/default-source/content2/roadway/ppmmanual/2017/volume1/chap33.pdf?sfvrsn=8bbdab3d_0; Queensland Government – Department of Transport and Main Roads Guide|https://www.tmr.qld.gov.au/_/media/busind/techstdpubs/hydraulics-and-drainage/road-drainage-manual/chapter9.pdf?sc_lang=en&amp;hash=AA6B9000678F92BC28393CEF043F02CF; Wisconsin DOT manual|https://wisconsindot.gov/dtsdManuals/strct/manuals/bridge/ch36.pdf</t>
-  </si>
-  <si>
     <t>IT Transport Guide|https://drive.google.com/file/d/11ptavSSCDtjiI6auCW3FEfp-auJEVloY/view?usp=drive_link</t>
   </si>
   <si>
@@ -309,9 +306,6 @@
     <t>Steel cables</t>
   </si>
   <si>
-    <t>Reinforced concrete</t>
-  </si>
-  <si>
     <t>Timber logs</t>
   </si>
   <si>
@@ -423,12 +417,6 @@
     <t>Iowa DOT Guide|https://iowadot.gov/research/reports/Year/2003andolder/fullreports/tr453.pdf</t>
   </si>
   <si>
-    <t>;Pedestrians, Bicyclists, Motorcyclists &amp; Pack animals (4kpa)</t>
-  </si>
-  <si>
-    <t>;Pedestrians, Bicyclists, Motorcyclists &amp; Pack animals (4kpa); Passenger Cars (10kpa); Heavy Commercial Vehicles (20kpa)</t>
-  </si>
-  <si>
     <t>Additional Material requirements</t>
   </si>
   <si>
@@ -495,9 +483,6 @@
     <t>Greater than</t>
   </si>
   <si>
-    <t>Masonry Arch Bridge; Box Culvert; Suspended Cable Bridge; Suspension Bridge</t>
-  </si>
-  <si>
     <t>Timber Log Footbridge</t>
   </si>
   <si>
@@ -513,15 +498,9 @@
     <t>Span &gt; 20m?</t>
   </si>
   <si>
-    <t>Masonry Arch Bridge; Suspended Cable Bridge; Suspension Bridge; Timber Log Footbridge</t>
-  </si>
-  <si>
     <t>Suspended Cable Bridge; Suspension Bridge; Timber Log Footbridge</t>
   </si>
   <si>
-    <t>Masonry Arch Bridge; Box Culvert</t>
-  </si>
-  <si>
     <t>Type of variable</t>
   </si>
   <si>
@@ -604,6 +583,87 @@
   </si>
   <si>
     <t>Unit cost</t>
+  </si>
+  <si>
+    <t>Reinforced Concrete</t>
+  </si>
+  <si>
+    <t>Masonry Stone Arch Bridge; Box Culvert; Suspended Cable Bridge; Suspension Bridge</t>
+  </si>
+  <si>
+    <t>Masonry Stone Arch Bridge; Suspended Cable Bridge; Suspension Bridge; Timber Log Footbridge</t>
+  </si>
+  <si>
+    <t>Masonry Stone Arch Bridge; Box Culvert</t>
+  </si>
+  <si>
+    <t>Labour intensity</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Is it a inherently labour intensive process, i.e., where the construction process cannot be made significantly faster or more efficient by improved manufacturing technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is a significantly long service life required, i.e. longer than 5 years? </t>
+  </si>
+  <si>
+    <t>Ontario Ministry of Transport Guide|http://www.bv.transports.gouv.qc.ca/mono/1165314.pdf; Florida DOT manual|https://fdotwww.blob.core.windows.net/sitefinity/docs/default-source/content2/roadway/ppmmanual/2017/volume1/chap33.pdf?sfvrsn=8bbdab3d_0; Queensland Government – Department of Transport and Main Roads Guide|https://www.tmr.qld.gov.au/_/media/busind/techstdpubs/hydraulics-and-drainage/road-drainage-manual/chapter9.pdf?sc_lang=enandhash=AA6B9000678F92BC28393CEF043F02CF; Wisconsin DOT manual|https://wisconsindot.gov/dtsdManuals/strct/manuals/bridge/ch36.pdf</t>
+  </si>
+  <si>
+    <t>;Pedestrians, Bicyclists, Motorcyclists and Pack animals : 4kpa</t>
+  </si>
+  <si>
+    <t>;Pedestrians, Bicyclists, Motorcyclists and Pack animals : 4kpa; Passenger Cars : 10kpa; Heavy Commercial Vehicles : 20kpa</t>
+  </si>
+  <si>
+    <t>Annual flooding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the river flood on average &gt; 10 times per year? </t>
+  </si>
+  <si>
+    <t>Masonry Stone Arch Bridge; Suspended Cable Bridge; Suspension Bridge; Timber Log Footbridge; Box Culvert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the average duration of traffic interruption per occurrence &gt; 3 days? </t>
+  </si>
+  <si>
+    <t>Road network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the alternative itinerary by an alternate route longer by more than 2 hours? </t>
+  </si>
+  <si>
+    <t>Wider Transport Network</t>
+  </si>
+  <si>
+    <t>Much longer by alternate route?</t>
+  </si>
+  <si>
+    <t>Long traffic interruptions?</t>
+  </si>
+  <si>
+    <t>Frequent flooding?</t>
+  </si>
+  <si>
+    <t>Labour intensive construction process?</t>
+  </si>
+  <si>
+    <t>Long Service Life Required?</t>
+  </si>
+  <si>
+    <t>Suspension Bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the Average Daily Traffic at the crossing point &lt; 200 vehicles. </t>
+  </si>
+  <si>
+    <t>Low Traffic?</t>
+  </si>
+  <si>
+    <t>Tower System</t>
   </si>
 </sst>
 </file>
@@ -878,7 +938,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -936,11 +996,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1222,651 +1283,708 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="37.42578125" style="29" customWidth="1"/>
-    <col min="5" max="6" width="39.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="39.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="39.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="39.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="39.140625" style="8" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="5"/>
+    <col min="5" max="7" width="39.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="39.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="39.28515625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="39.140625" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17"/>
       <c r="B1" s="24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="I1" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" s="33" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="B4" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="29" t="s">
+      <c r="I5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="B6" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="H6" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="G6" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="I11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>106</v>
+        <v>16</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="F14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="5">
         <v>120</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="5">
+        <v>120</v>
+      </c>
+      <c r="G16" s="11">
         <v>20</v>
       </c>
-      <c r="G16" s="5">
+      <c r="H16" s="5">
         <v>15</v>
       </c>
-      <c r="H16" s="12">
+      <c r="I16" s="12">
         <v>80</v>
       </c>
-      <c r="I16" s="8">
+      <c r="J16" s="8">
         <v>20</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K16" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="10" t="s">
+      <c r="I24" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>107</v>
-      </c>
       <c r="J24" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" display="http://nepaltrailbridges.org.np/upload/upload/files/Download/D%20Type%20Handbook.pdf"/>
+    <hyperlink ref="F4" r:id="rId2" display="http://nepaltrailbridges.org.np/upload/upload/files/Download/D%20Type%20Handbook.pdf"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1883,175 +2001,175 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="40"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="37"/>
+      <c r="A15" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="40"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="37"/>
+      <c r="A25" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="40"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2069,8 +2187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,132 +2202,132 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="H4" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D5" s="36">
         <v>0.02</v>
       </c>
       <c r="E5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2220,10 +2338,174 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18" style="5" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,30 +2515,30 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B2">
-        <v>115000</v>
+        <v>128000</v>
       </c>
       <c r="C2">
         <f>B2*0.00089</f>
-        <v>102.35</v>
+        <v>113.91999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2268,7 +2550,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2280,7 +2562,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2292,14 +2574,14 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B6">
-        <v>250000</v>
+        <v>275000</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>222.5</v>
+        <v>244.75</v>
       </c>
     </row>
   </sheetData>
@@ -2308,12 +2590,102 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2">
+        <v>115000</v>
+      </c>
+      <c r="C2">
+        <f>B2*0.00089</f>
+        <v>102.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3">
+        <v>70000</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C6" si="0">B3*0.00089</f>
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4">
+        <v>15000</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>13.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5">
+        <v>15000</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>13.35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6">
+        <v>250000</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>222.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,20 +2697,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="38">
+      <c r="A2" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="37">
         <v>10700000</v>
       </c>
       <c r="C2">
@@ -2348,14 +2720,27 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="38">
+        <v>159</v>
+      </c>
+      <c r="B3" s="37">
         <v>820000</v>
       </c>
       <c r="C3">
         <f>B3*0.00089</f>
         <v>729.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="37">
+        <f>8200000 + 4000000</f>
+        <v>12200000</v>
+      </c>
+      <c r="C4">
+        <f>B4*0.00089</f>
+        <v>10858</v>
       </c>
     </row>
   </sheetData>
@@ -2363,11 +2748,66 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="37">
+        <v>10700000</v>
+      </c>
+      <c r="C2">
+        <f>B2*0.00089</f>
+        <v>9523</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="37">
+        <v>820000</v>
+      </c>
+      <c r="C3">
+        <f>B3*0.00089</f>
+        <v>729.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2378,15 +2818,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -2394,7 +2834,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B3">
         <v>1.4</v>
@@ -2402,7 +2842,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -2410,7 +2850,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -2418,7 +2858,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -2426,7 +2866,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -2434,7 +2874,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B8">
         <v>4</v>

</xml_diff>

<commit_message>
Modified table in information synthesis tab
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -303,15 +303,6 @@
     <t>Principle structural material</t>
   </si>
   <si>
-    <t>Steel cables</t>
-  </si>
-  <si>
-    <t>Timber logs</t>
-  </si>
-  <si>
-    <t>Structural timber members</t>
-  </si>
-  <si>
     <t>Structural form</t>
   </si>
   <si>
@@ -372,9 +363,6 @@
     <t>Masonry Stone Arch Bridge</t>
   </si>
   <si>
-    <t>Masonry stone</t>
-  </si>
-  <si>
     <t xml:space="preserve">BTC Uganda Manual|https://roadsforwater.org/wp-content/uploads/2022/12/Manual-stone-arch-bridges-final.pdf </t>
   </si>
   <si>
@@ -396,21 +384,6 @@
     <t>Span (m)</t>
   </si>
   <si>
-    <t>;Rigid, non-rigid; Three sided/Open footing/ Slab culvert, Four Sided; Arch topped, Rectangular</t>
-  </si>
-  <si>
-    <t>;Beam type; Truss type</t>
-  </si>
-  <si>
-    <t>;Roman arch (single/multiple); Segmental arch (single/multiple); Arch culvert (single/multiple)</t>
-  </si>
-  <si>
-    <t>;Assembled on site</t>
-  </si>
-  <si>
-    <t>;Built on site</t>
-  </si>
-  <si>
     <t>Low Water Crossing Structure</t>
   </si>
   <si>
@@ -450,18 +423,6 @@
     <t>Laying concrete; Concrete block/Cinder block construction; Fixing and tying steel rebar (minimal)</t>
   </si>
   <si>
-    <t>; Reinforced Concrete; Concrete Blocks; Earth and gravels; Gabions</t>
-  </si>
-  <si>
-    <t>;Built on site ;Assembled on site ;Prefabricated ;Incremental Launch</t>
-  </si>
-  <si>
-    <t>;Built on site ;Assembled on site</t>
-  </si>
-  <si>
-    <t>;Precast ;Cast in-situ</t>
-  </si>
-  <si>
     <t>Decision Question</t>
   </si>
   <si>
@@ -585,9 +546,6 @@
     <t>Unit cost</t>
   </si>
   <si>
-    <t>Reinforced Concrete</t>
-  </si>
-  <si>
     <t>Masonry Stone Arch Bridge; Box Culvert; Suspended Cable Bridge; Suspension Bridge</t>
   </si>
   <si>
@@ -612,12 +570,6 @@
     <t>Ontario Ministry of Transport Guide|http://www.bv.transports.gouv.qc.ca/mono/1165314.pdf; Florida DOT manual|https://fdotwww.blob.core.windows.net/sitefinity/docs/default-source/content2/roadway/ppmmanual/2017/volume1/chap33.pdf?sfvrsn=8bbdab3d_0; Queensland Government – Department of Transport and Main Roads Guide|https://www.tmr.qld.gov.au/_/media/busind/techstdpubs/hydraulics-and-drainage/road-drainage-manual/chapter9.pdf?sc_lang=enandhash=AA6B9000678F92BC28393CEF043F02CF; Wisconsin DOT manual|https://wisconsindot.gov/dtsdManuals/strct/manuals/bridge/ch36.pdf</t>
   </si>
   <si>
-    <t>;Pedestrians, Bicyclists, Motorcyclists and Pack animals : 4kpa</t>
-  </si>
-  <si>
-    <t>;Pedestrians, Bicyclists, Motorcyclists and Pack animals : 4kpa; Passenger Cars : 10kpa; Heavy Commercial Vehicles : 20kpa</t>
-  </si>
-  <si>
     <t>Annual flooding</t>
   </si>
   <si>
@@ -664,6 +616,54 @@
   </si>
   <si>
     <t>Tower System</t>
+  </si>
+  <si>
+    <t>- Reinforced Concrete; Concrete Blocks; Earth and gravels; Gabions</t>
+  </si>
+  <si>
+    <t>- Built on site ; Assembled on site</t>
+  </si>
+  <si>
+    <t>- Pedestrians, Bicyclists, Motorcyclists and Pack animals : 4kpa; Passenger Cars : 10kpa; Heavy Commercial Vehicles : 20kpa</t>
+  </si>
+  <si>
+    <t>- Pedestrians, Bicyclists, Motorcyclists and Pack animals : 4kpa</t>
+  </si>
+  <si>
+    <t>- Built on site ;Assembled on site ;Prefabricated ;Incremental Launch</t>
+  </si>
+  <si>
+    <t>- Precast ;Cast in-situ</t>
+  </si>
+  <si>
+    <t>- Built on site</t>
+  </si>
+  <si>
+    <t>- Roman arch (single/multiple); Segmental arch (single/multiple); Arch culvert (single/multiple)</t>
+  </si>
+  <si>
+    <t>- Beam type; Truss type</t>
+  </si>
+  <si>
+    <t>- Rigid, non-rigid; Three sided/Open footing/ Slab culvert, Four Sided; Arch topped, Rectangular</t>
+  </si>
+  <si>
+    <t>- Assembled on site</t>
+  </si>
+  <si>
+    <t>- Masonry stone</t>
+  </si>
+  <si>
+    <t>- Structural timber members</t>
+  </si>
+  <si>
+    <t>- Reinforced Concrete</t>
+  </si>
+  <si>
+    <t>- Timber logs</t>
+  </si>
+  <si>
+    <t>- Steel cables</t>
   </si>
 </sst>
 </file>
@@ -938,7 +938,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1002,6 +1002,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1285,11 +1286,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,27 +1320,27 @@
         <v>7</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>8</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K1" s="33" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>20</v>
@@ -1348,28 +1349,28 @@
         <v>20</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>85</v>
-      </c>
       <c r="J2" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1385,26 +1386,26 @@
       <c r="D3" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>126</v>
+      <c r="E3" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1430,16 +1431,16 @@
         <v>38</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>42</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1465,16 +1466,16 @@
         <v>47</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1492,14 +1493,14 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="H6" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>110</v>
+      <c r="H6" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1532,26 +1533,26 @@
       <c r="D8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>128</v>
+      <c r="E8" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1567,26 +1568,26 @@
       <c r="D9" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>181</v>
+      <c r="E9" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1609,22 +1610,22 @@
         <v>66</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>75</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>24</v>
@@ -1697,10 +1698,10 @@
         <v>29</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1741,12 +1742,12 @@
         <v>32</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>20</v>
@@ -1859,7 +1860,7 @@
         <v>23</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1892,7 +1893,7 @@
     </row>
     <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>20</v>
@@ -1910,48 +1911,48 @@
         <v>13</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>28</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="10" t="s">
+      <c r="I24" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>90</v>
-      </c>
       <c r="J24" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2129,7 +2130,7 @@
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="40" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B25" s="40"/>
     </row>
@@ -2143,33 +2144,33 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2202,132 +2203,132 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="H2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="H4" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D5" s="36">
         <v>0.02</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="G5" s="34" t="s">
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2340,8 +2341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2356,59 +2357,59 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>143</v>
-      </c>
       <c r="E1" s="33" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>8</v>
@@ -2416,82 +2417,82 @@
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2515,18 +2516,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B2">
         <v>128000</v>
@@ -2538,7 +2539,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2550,7 +2551,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2562,7 +2563,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2574,7 +2575,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B6">
         <v>275000</v>
@@ -2605,18 +2606,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B2">
         <v>115000</v>
@@ -2628,7 +2629,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2640,7 +2641,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2652,7 +2653,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2664,7 +2665,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B6">
         <v>250000</v>
@@ -2697,18 +2698,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B2" s="37">
         <v>10700000</v>
@@ -2720,7 +2721,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B3" s="37">
         <v>820000</v>
@@ -2732,7 +2733,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="B4" s="37">
         <f>8200000 + 4000000</f>
@@ -2765,18 +2766,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B2" s="37">
         <v>10700000</v>
@@ -2788,7 +2789,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B3" s="37">
         <v>820000</v>
@@ -2818,15 +2819,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -2834,7 +2835,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B3">
         <v>1.4</v>
@@ -2842,7 +2843,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -2850,7 +2851,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -2858,7 +2859,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -2866,7 +2867,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -2874,7 +2875,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B8">
         <v>4</v>

</xml_diff>

<commit_message>
Life cycle cost, road safety impacts removed
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -23,7 +23,7 @@
     <sheet name="Default Unit Costs" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$I$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$I$23</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="196">
   <si>
     <t>Construction method</t>
   </si>
@@ -85,12 +85,6 @@
   </si>
   <si>
     <t>River flow</t>
-  </si>
-  <si>
-    <t>Life cycle cost</t>
-  </si>
-  <si>
-    <t>Road safety impacts</t>
   </si>
   <si>
     <t>Suspended Cable Bridge</t>
@@ -1284,13 +1278,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,213 +1302,213 @@
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17"/>
       <c r="B1" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K1" s="33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="27" t="s">
+      <c r="F2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>82</v>
-      </c>
       <c r="J2" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="F5" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="H6" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I6" s="41" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1525,151 +1519,151 @@
         <v>0</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G8" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="H8" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>188</v>
-      </c>
       <c r="K8" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1677,51 +1671,51 @@
         <v>1</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G14" s="10"/>
     </row>
@@ -1730,33 +1724,33 @@
         <v>2</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E16" s="5">
         <v>120</v>
@@ -1777,44 +1771,44 @@
         <v>20</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1822,19 +1816,19 @@
         <v>3</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1842,141 +1836,113 @@
         <v>4</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2009,168 +1975,168 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B15" s="40"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="40" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B25" s="40"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2203,132 +2169,132 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>119</v>
-      </c>
       <c r="G1" s="35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
         <v>125</v>
       </c>
-      <c r="B3" t="s">
-        <v>127</v>
-      </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D5" s="36">
         <v>0.02</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2357,142 +2323,142 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>119</v>
-      </c>
       <c r="F1" s="33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>163</v>
-      </c>
       <c r="D3" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>168</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>168</v>
-      </c>
       <c r="F5" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>172</v>
-      </c>
       <c r="E6" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>172</v>
-      </c>
       <c r="E7" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2516,18 +2482,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B2">
         <v>128000</v>
@@ -2539,7 +2505,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2551,7 +2517,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2563,7 +2529,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2575,7 +2541,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B6">
         <v>275000</v>
@@ -2606,18 +2572,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B2">
         <v>115000</v>
@@ -2629,7 +2595,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2641,7 +2607,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2653,7 +2619,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2665,7 +2631,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B6">
         <v>250000</v>
@@ -2698,18 +2664,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B2" s="37">
         <v>10700000</v>
@@ -2721,7 +2687,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B3" s="37">
         <v>820000</v>
@@ -2733,7 +2699,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B4" s="37">
         <f>8200000 + 4000000</f>
@@ -2766,18 +2732,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B2" s="37">
         <v>10700000</v>
@@ -2789,7 +2755,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B3" s="37">
         <v>820000</v>
@@ -2819,15 +2785,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -2835,7 +2801,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B3">
         <v>1.4</v>
@@ -2843,7 +2809,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -2851,7 +2817,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -2859,7 +2825,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -2867,7 +2833,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -2875,7 +2841,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B8">
         <v>4</v>

</xml_diff>

<commit_message>
Images moved to pages folder
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8415" windowHeight="3225"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -204,12 +204,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>C:\Users\mwendwa.kiko\Documents\Personal_Kiko\E4C_Internship\Other_Docs\Dashboard_test\Utils\Images\Suspended Cable Bridge.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\mwendwa.kiko\Documents\Personal_Kiko\E4C_Internship\Other_Docs\Dashboard_test\Utils\Images\Timber Log Footbridge.jpg</t>
-  </si>
-  <si>
     <t>Segmental Construction</t>
   </si>
   <si>
@@ -348,12 +342,6 @@
     <t xml:space="preserve">A vented ford is in a mix of compression and flexure, but we'll nonetheless ignore that. </t>
   </si>
   <si>
-    <t>C:\Users\mwendwa.kiko\Documents\Personal_Kiko\E4C_Internship\Other_Docs\Dashboard_test\Utils\Images\Box Culvert.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\mwendwa.kiko\Documents\Personal_Kiko\E4C_Internship\Other_Docs\Dashboard_test\Utils\Images\Sawn Timber Bridge.jpg</t>
-  </si>
-  <si>
     <t>Masonry Stone Arch Bridge</t>
   </si>
   <si>
@@ -372,9 +360,6 @@
     <t>Maximum traffic load of 40 tons for Roman Arch Bridge and 15 tons for segmental arch bridge.</t>
   </si>
   <si>
-    <t>C:\Users\mwendwa.kiko\Documents\Personal_Kiko\E4C_Internship\Other_Docs\Dashboard_test\Utils\Images\Stone Masonry Bridge.jpg</t>
-  </si>
-  <si>
     <t>Span (m)</t>
   </si>
   <si>
@@ -393,9 +378,6 @@
     <t>Approach grades should be less than 10%; Height between road approach and LWSC surface should be less than 12 ft (3.6m)</t>
   </si>
   <si>
-    <t>C:\Users\mwendwa.kiko\Documents\Personal_Kiko\E4C_Internship\Other_Docs\Dashboard_test\Utils\Images\Concrete_Ford.JPG</t>
-  </si>
-  <si>
     <t>Unvented Ford/Drift</t>
   </si>
   <si>
@@ -658,6 +640,24 @@
   </si>
   <si>
     <t>- Steel cables</t>
+  </si>
+  <si>
+    <t>Suspended Cable Bridge.jpg</t>
+  </si>
+  <si>
+    <t>Timber Log Footbridge.jpg</t>
+  </si>
+  <si>
+    <t>Box Culvert.jpg</t>
+  </si>
+  <si>
+    <t>Sawn Timber Bridge.jpg</t>
+  </si>
+  <si>
+    <t>Stone Masonry Bridge.jpg</t>
+  </si>
+  <si>
+    <t>Concrete_Ford.JPG</t>
   </si>
 </sst>
 </file>
@@ -1281,10 +1281,10 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,27 +1314,27 @@
         <v>5</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="K1" s="33" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>18</v>
@@ -1343,33 +1343,33 @@
         <v>22</v>
       </c>
       <c r="D2" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>80</v>
-      </c>
       <c r="J2" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>18</v>
@@ -1381,25 +1381,25 @@
         <v>22</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1425,19 +1425,19 @@
         <v>36</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>40</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>42</v>
       </c>
@@ -1451,25 +1451,25 @@
         <v>22</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>44</v>
+        <v>190</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>44</v>
+        <v>190</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>45</v>
+        <v>191</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>92</v>
+        <v>192</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>100</v>
+        <v>194</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>107</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1488,13 +1488,13 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="H6" s="12" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1528,25 +1528,25 @@
         <v>22</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1563,30 +1563,30 @@
         <v>22</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>22</v>
@@ -1598,28 +1598,28 @@
         <v>22</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>22</v>
@@ -1692,10 +1692,10 @@
         <v>27</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1736,12 +1736,12 @@
         <v>30</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>18</v>
@@ -1854,12 +1854,12 @@
         <v>21</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B21" s="30" t="s">
         <v>18</v>
@@ -1877,48 +1877,48 @@
         <v>11</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>26</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="10" t="s">
+      <c r="H22" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="10" t="s">
+      <c r="I22" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H22" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>85</v>
-      </c>
       <c r="J22" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1975,73 +1975,73 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -2052,91 +2052,91 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B25" s="41"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2169,132 +2169,132 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G3" s="34" t="s">
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>127</v>
-      </c>
       <c r="G4" s="34" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="H4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D5" s="36">
         <v>0.02</v>
       </c>
       <c r="E5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="G5" s="34" t="s">
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2323,59 +2323,59 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>6</v>
@@ -2383,82 +2383,82 @@
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2482,18 +2482,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B2">
         <v>128000</v>
@@ -2505,7 +2505,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2517,7 +2517,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2529,7 +2529,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2541,7 +2541,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B6">
         <v>275000</v>
@@ -2572,18 +2572,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B2">
         <v>115000</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2619,7 +2619,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2631,7 +2631,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B6">
         <v>250000</v>
@@ -2664,18 +2664,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B2" s="37">
         <v>10700000</v>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B3" s="37">
         <v>820000</v>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B4" s="37">
         <f>8200000 + 4000000</f>
@@ -2732,18 +2732,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B2" s="37">
         <v>10700000</v>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B3" s="37">
         <v>820000</v>
@@ -2785,15 +2785,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -2801,7 +2801,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B3">
         <v>1.4</v>
@@ -2809,7 +2809,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -2817,7 +2817,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -2825,7 +2825,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -2833,7 +2833,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B8">
         <v>4</v>

</xml_diff>

<commit_message>
Suspension bridge image changed, images removed from pages folder
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="197">
   <si>
     <t>Construction method</t>
   </si>
@@ -658,6 +658,9 @@
   </si>
   <si>
     <t>Concrete_Ford.JPG</t>
+  </si>
+  <si>
+    <t>Helvetas_Bridge.jpg</t>
   </si>
 </sst>
 </file>
@@ -1281,10 +1284,10 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1457,7 @@
         <v>190</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>191</v>

</xml_diff>

<commit_message>
Span no longer a feasibility criterion
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -1284,10 +1284,10 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,7 +1750,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Span no longer for comparison
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -1284,10 +1284,10 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1747,7 +1747,7 @@
         <v>96</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C16" s="31" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Suspended bridge, suspension bridge climate risk reevaluated.
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -105,9 +105,6 @@
     <t>span/25</t>
   </si>
   <si>
-    <t>Vulnerable to rises in river level, because of low freeboard due to sag</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wheel cable saddle: 4 pieces; Roofing tar: 1 gallon; 75mm dia flexible plastic tubing: 250cm per cable; 50mm dia flexible plastic tubing: 110cm per cable; Tie wire: 10kg; Lag screw - 10mm x 7.5cm long: 5-6 per deck panel + 4 per crossbeam if using nailer; Lag screw - 10mm x 5cm long: 12 if center cable is used; 20cm x 5cm x 10cm wood cable guide: 6 if center cable used; Galvanized tie wire: 5kg; </t>
   </si>
   <si>
@@ -661,6 +658,9 @@
   </si>
   <si>
     <t>Span (m)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usually have a high freeboard, therefore less vulnerable than other bridge types to increases in river level because of climate change. </t>
   </si>
 </sst>
 </file>
@@ -996,10 +996,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1287,7 +1287,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,104 +1305,104 @@
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16"/>
       <c r="B1" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J1" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K1" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="26" t="s">
+      <c r="E2" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>76</v>
-      </c>
       <c r="I2" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I3" s="39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1410,108 +1410,108 @@
         <v>7</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="K5" s="8" t="s">
         <v>193</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="H6" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I6" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1522,34 +1522,34 @@
         <v>0</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G8" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="H8" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="I8" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="K8" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1557,96 +1557,96 @@
         <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="F10" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1654,19 +1654,19 @@
         <v>9</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1674,51 +1674,51 @@
         <v>1</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="F14" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G14" s="10"/>
     </row>
@@ -1727,33 +1727,33 @@
         <v>2</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="5">
         <v>120</v>
@@ -1761,7 +1761,7 @@
       <c r="F16" s="5">
         <v>120</v>
       </c>
-      <c r="G16" s="41">
+      <c r="G16" s="40">
         <v>20</v>
       </c>
       <c r="H16" s="5">
@@ -1774,44 +1774,44 @@
         <v>20</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1819,13 +1819,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>10</v>
@@ -1839,109 +1839,109 @@
         <v>4</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="I21" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="10" t="s">
+      <c r="F22" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="G22" s="10" t="s">
+      <c r="H22" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="I22" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>83</v>
-      </c>
       <c r="J22" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="F23" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1971,175 +1971,175 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="41"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="40"/>
+      <c r="B15" s="41"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="40"/>
+      <c r="A25" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="41"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2172,132 +2172,132 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>110</v>
-      </c>
       <c r="G1" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>115</v>
-      </c>
       <c r="H2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" s="33" t="s">
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" s="35">
         <v>0.02</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G5" s="33" t="s">
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2326,59 +2326,59 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>110</v>
-      </c>
       <c r="F1" s="32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>6</v>
@@ -2386,82 +2386,82 @@
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>163</v>
-      </c>
       <c r="E6" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2485,18 +2485,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2">
         <v>128000</v>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2520,7 +2520,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2532,7 +2532,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6">
         <v>275000</v>
@@ -2575,18 +2575,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2">
         <v>115000</v>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6">
         <v>250000</v>
@@ -2667,18 +2667,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="36">
         <v>10700000</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="36">
         <v>820000</v>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" s="36">
         <f>8200000 + 4000000</f>
@@ -2735,18 +2735,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="36">
         <v>10700000</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="36">
         <v>820000</v>
@@ -2788,15 +2788,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -2804,7 +2804,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3">
         <v>1.4</v>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -2828,7 +2828,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -2836,7 +2836,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8">
         <v>4</v>

</xml_diff>

<commit_message>
Excess info trimmed from info synthesis tab
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8415" windowHeight="3225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8412" windowHeight="3228" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Default Unit Costs" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$I$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$I$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +40,7 @@
     <author>Mwendwa KIKO</author>
   </authors>
   <commentList>
-    <comment ref="H16" authorId="0" shapeId="0">
+    <comment ref="H13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,14 +70,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="178">
   <si>
     <t>Construction method</t>
   </si>
   <si>
-    <t>Human capital requirements</t>
-  </si>
-  <si>
     <t>River channel profile</t>
   </si>
   <si>
@@ -105,15 +102,9 @@
     <t>span/25</t>
   </si>
   <si>
-    <t xml:space="preserve">Wheel cable saddle: 4 pieces; Roofing tar: 1 gallon; 75mm dia flexible plastic tubing: 250cm per cable; 50mm dia flexible plastic tubing: 110cm per cable; Tie wire: 10kg; Lag screw - 10mm x 7.5cm long: 5-6 per deck panel + 4 per crossbeam if using nailer; Lag screw - 10mm x 5cm long: 12 if center cable is used; 20cm x 5cm x 10cm wood cable guide: 6 if center cable used; Galvanized tie wire: 5kg; </t>
-  </si>
-  <si>
     <t xml:space="preserve">U-nails/staples: 1kg x span/10; Fencing - 1.2m (4') tall: span x 2; </t>
   </si>
   <si>
-    <t>Minimal bridge design experience required if one remains within the limits of the B2P suspension bridge manual. Some structural engineering knowledge is still required to be able to interpret design requirements; size elements; etc.</t>
-  </si>
-  <si>
     <t>5m freeboard minimum required; To protect the bridge from over-flooding and strong erosion, the bridge site should not be located near the confluence of two rivers</t>
   </si>
   <si>
@@ -126,12 +117,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Timber logs, preferably hardwood; 7-10cm diameter poles nailed across stringers to make a deck; Optional handrails; Reinforced concrete for end stub columns and their bases</t>
-  </si>
-  <si>
-    <t>Labour intensive. Requires manual labour for positioning the logs, nailing the stringers, putting the bridge in place.  </t>
-  </si>
-  <si>
     <t>Low acceptable flow volumes, due to low freeboard</t>
   </si>
   <si>
@@ -150,15 +135,6 @@
     <t>Particularly sensitive to wetness, therefore covering or other measures needed to make them less sensitive to increased rainfall due to climate change. </t>
   </si>
   <si>
-    <t>Skilled carpenters</t>
-  </si>
-  <si>
-    <t>Permitted hardwood and softwood sections; Reinforced concrete abutments; Steel Connections; Guardrail</t>
-  </si>
-  <si>
-    <t>Reinforced concrete (Minimum Class 25); Reinforcing steel (Minimum yield strength 460)</t>
-  </si>
-  <si>
     <t>Four sided box culverts typically used where the streambed is earth or granular soil and rock is not close enough to the streambed to directly support the structure</t>
   </si>
   <si>
@@ -168,9 +144,6 @@
     <t>2% max slope of streambed without stepped footing</t>
   </si>
   <si>
-    <t>Basic Layout (where there is one)</t>
-  </si>
-  <si>
     <t>Human capital requirements - dimension dependent</t>
   </si>
   <si>
@@ -306,21 +279,6 @@
     <t>Flexure Type; Truss Type</t>
   </si>
   <si>
-    <t>Upskilling Human Resources</t>
-  </si>
-  <si>
-    <t>Fixing and tying steel rebar (minimal); Laying concrete (minimal); Cable fixing; Carpentry (minimal)</t>
-  </si>
-  <si>
-    <t>Forestry (logging, harvesting, transporting timber); Fixing and tying steel rebar (minimal); Laying concrete (minimal); Carpentry</t>
-  </si>
-  <si>
-    <t>Fixing and tying steel rebar; Laying concrete; Carpentry</t>
-  </si>
-  <si>
-    <t>Forestry (logging, harvesting, transporting timber) - minimal; Fixing and tying steel rebar (minimal); Laying concrete (minimal); Carpentry</t>
-  </si>
-  <si>
     <t>Structural Form</t>
   </si>
   <si>
@@ -348,12 +306,6 @@
     <t>Service life of 3-5 years without treatment</t>
   </si>
   <si>
-    <t xml:space="preserve">Labour intensive: requires unskilled workers to collect stones and sand, masons to build bridge, carpenters to construct scaffolding.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masonry skills: Cutting, dressing and laying stones, reading blueprints, etc; Carpentry skills and knowledge. </t>
-  </si>
-  <si>
     <t>Maximum traffic load of 40 tons for Roman Arch Bridge and 15 tons for segmental arch bridge.</t>
   </si>
   <si>
@@ -363,9 +315,6 @@
     <t>Iowa DOT Guide|https://iowadot.gov/research/reports/Year/2003andolder/fullreports/tr453.pdf</t>
   </si>
   <si>
-    <t>Additional Material requirements</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stream channel should be stable. </t>
   </si>
   <si>
@@ -378,9 +327,6 @@
     <t>Max flow depth of 6 inches (15.2cm)</t>
   </si>
   <si>
-    <t xml:space="preserve">Depends on construction method: Assembly on site from concrete blocks more labour intensive than reinforced concrete construction. </t>
-  </si>
-  <si>
     <t>Climate risks</t>
   </si>
   <si>
@@ -388,9 +334,6 @@
   </si>
   <si>
     <t xml:space="preserve">Vulnerable to rise in normal flow level, or to increased occurrences of flooding, since this would render them unusable for extended periods of time. </t>
-  </si>
-  <si>
-    <t>Laying concrete; Concrete block/Cinder block construction; Fixing and tying steel rebar (minimal)</t>
   </si>
   <si>
     <t>Decision Question</t>
@@ -667,7 +610,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,12 +629,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -935,19 +872,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -956,19 +892,19 @@
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -979,25 +915,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1281,671 +1217,558 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="37.42578125" style="28" customWidth="1"/>
-    <col min="5" max="7" width="39.42578125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="39.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="39.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="39.28515625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="39.140625" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="5"/>
+    <col min="1" max="1" width="37.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="37.44140625" style="27" customWidth="1"/>
+    <col min="5" max="7" width="39.44140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="39.109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="39.33203125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="39.109375" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="11.44140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16"/>
-      <c r="B1" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="14" t="s">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15"/>
+      <c r="B1" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="I1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="H1" s="14" t="s">
+      <c r="F3" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="B4" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="25" t="s">
+      <c r="K4" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="I3" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>21</v>
+      <c r="B6" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>16</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="H6" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="I6" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="27" t="s">
+      <c r="H6" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="G8" s="11" t="s">
+      <c r="K12" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="B13" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="5">
+        <v>120</v>
+      </c>
+      <c r="F13" s="5">
+        <v>120</v>
+      </c>
+      <c r="G13" s="39">
+        <v>20</v>
+      </c>
+      <c r="H13" s="5">
+        <v>15</v>
+      </c>
+      <c r="I13" s="10">
+        <v>80</v>
+      </c>
+      <c r="J13" s="8">
+        <v>20</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="F18" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="B19" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="5">
-        <v>120</v>
-      </c>
-      <c r="F16" s="5">
-        <v>120</v>
-      </c>
-      <c r="G16" s="40">
-        <v>20</v>
-      </c>
-      <c r="H16" s="5">
-        <v>15</v>
-      </c>
-      <c r="I16" s="11">
-        <v>80</v>
-      </c>
-      <c r="J16" s="8">
-        <v>20</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1964,182 +1787,182 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="40"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="40"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="3" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="3" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="3" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="41"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="B22" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A25" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="40"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="41"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B28" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2161,143 +1984,143 @@
       <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" style="33" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" style="33" customWidth="1"/>
+    <col min="4" max="5" width="24.109375" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="35.44140625" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>125</v>
+        <v>92</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>106</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>116</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>114</v>
+        <v>94</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>6</v>
+        <v>94</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>150</v>
+        <v>94</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>131</v>
       </c>
       <c r="H4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="35">
+        <v>103</v>
+      </c>
+      <c r="D5" s="34">
         <v>0.02</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>6</v>
+        <v>94</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2314,154 +2137,154 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" style="8" customWidth="1"/>
     <col min="4" max="4" width="18" style="5" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>170</v>
-      </c>
       <c r="B7" s="8" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2478,25 +2301,25 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B2">
         <v>128000</v>
@@ -2506,9 +2329,9 @@
         <v>113.91999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2518,9 +2341,9 @@
         <v>62.3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2530,9 +2353,9 @@
         <v>13.35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2542,9 +2365,9 @@
         <v>13.35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B6">
         <v>275000</v>
@@ -2564,29 +2387,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B2">
         <v>115000</v>
@@ -2596,9 +2419,9 @@
         <v>102.35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2608,9 +2431,9 @@
         <v>62.3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2620,9 +2443,9 @@
         <v>13.35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2632,9 +2455,9 @@
         <v>13.35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B6">
         <v>250000</v>
@@ -2658,29 +2481,29 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="36">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="35">
         <v>10700000</v>
       </c>
       <c r="C2">
@@ -2688,11 +2511,11 @@
         <v>9523</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" s="36">
+        <v>117</v>
+      </c>
+      <c r="B3" s="35">
         <v>820000</v>
       </c>
       <c r="C3">
@@ -2700,11 +2523,11 @@
         <v>729.8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="36">
+        <v>152</v>
+      </c>
+      <c r="B4" s="35">
         <f>8200000 + 4000000</f>
         <v>12200000</v>
       </c>
@@ -2726,29 +2549,29 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="36">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="35">
         <v>10700000</v>
       </c>
       <c r="C2">
@@ -2756,11 +2579,11 @@
         <v>9523</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" s="36">
+        <v>117</v>
+      </c>
+      <c r="B3" s="35">
         <v>820000</v>
       </c>
       <c r="C3">
@@ -2781,70 +2604,70 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B3">
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B4">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="B6">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="B8">
         <v>4</v>

</xml_diff>

<commit_message>
Excess info trimmed from info synthesis tab 2
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8412" windowHeight="3228" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8412" windowHeight="3228"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Default Unit Costs" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$I$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$I$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +40,7 @@
     <author>Mwendwa KIKO</author>
   </authors>
   <commentList>
-    <comment ref="H13" authorId="0" shapeId="0">
+    <comment ref="H11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="174">
   <si>
     <t>Construction method</t>
   </si>
@@ -96,15 +96,9 @@
     <t>Allowable Traffic</t>
   </si>
   <si>
-    <t>Material requirements - dimension dependent</t>
-  </si>
-  <si>
     <t>span/25</t>
   </si>
   <si>
-    <t xml:space="preserve">U-nails/staples: 1kg x span/10; Fencing - 1.2m (4') tall: span x 2; </t>
-  </si>
-  <si>
     <t>5m freeboard minimum required; To protect the bridge from over-flooding and strong erosion, the bridge site should not be located near the confluence of two rivers</t>
   </si>
   <si>
@@ -142,12 +136,6 @@
   </si>
   <si>
     <t>2% max slope of streambed without stepped footing</t>
-  </si>
-  <si>
-    <t>Human capital requirements - dimension dependent</t>
-  </si>
-  <si>
-    <t>Mandays for skilled labour: 1.3 x span + 400; Mandays for unskilled labour: 5 x span + 400</t>
   </si>
   <si>
     <t>IT Transport Guide|https://drive.google.com/file/d/11ptavSSCDtjiI6auCW3FEfp-auJEVloY/view?usp=drive_link</t>
@@ -1217,13 +1205,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,104 +1229,104 @@
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="K2" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -1346,94 +1334,94 @@
         <v>6</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="J4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="K5" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="H6" s="10" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I6" s="38" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1441,34 +1429,34 @@
         <v>0</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H7" s="38" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -1476,234 +1464,248 @@
         <v>7</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>16</v>
+    </row>
+    <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>14</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="E11" s="5">
+        <v>120</v>
+      </c>
+      <c r="F11" s="5">
+        <v>120</v>
+      </c>
+      <c r="G11" s="39">
+        <v>20</v>
+      </c>
+      <c r="H11" s="5">
+        <v>15</v>
+      </c>
+      <c r="I11" s="10">
+        <v>80</v>
+      </c>
+      <c r="J11" s="8">
+        <v>20</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G12" s="11"/>
       <c r="H12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="8" t="s">
-        <v>81</v>
-      </c>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>176</v>
+        <v>16</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="5">
-        <v>120</v>
-      </c>
-      <c r="F13" s="5">
-        <v>120</v>
-      </c>
-      <c r="G13" s="39">
-        <v>20</v>
-      </c>
-      <c r="H13" s="5">
-        <v>15</v>
-      </c>
-      <c r="I13" s="10">
+      <c r="G13" s="11"/>
+      <c r="H13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="J13" s="8">
-        <v>20</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+    </row>
+    <row r="16" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>16</v>
+      <c r="K16" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>14</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>11</v>
@@ -1711,64 +1713,9 @@
       <c r="F17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1801,73 +1748,73 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.35">
@@ -1878,91 +1825,91 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="40" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B25" s="40"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1995,132 +1942,132 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="F1" s="33" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G3" s="32" t="s">
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
         <v>99</v>
-      </c>
-      <c r="B4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" t="s">
-        <v>103</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D5" s="34">
         <v>0.02</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G5" s="32" t="s">
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2149,59 +2096,59 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>5</v>
@@ -2209,82 +2156,82 @@
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2308,18 +2255,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B2">
         <v>128000</v>
@@ -2331,7 +2278,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2343,7 +2290,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2355,7 +2302,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2367,7 +2314,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B6">
         <v>275000</v>
@@ -2387,7 +2334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -2398,18 +2345,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B2">
         <v>115000</v>
@@ -2421,7 +2368,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B3">
         <v>70000</v>
@@ -2433,7 +2380,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -2445,7 +2392,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B5">
         <v>15000</v>
@@ -2457,7 +2404,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B6">
         <v>250000</v>
@@ -2490,18 +2437,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B2" s="35">
         <v>10700000</v>
@@ -2513,7 +2460,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B3" s="35">
         <v>820000</v>
@@ -2525,7 +2472,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B4" s="35">
         <f>8200000 + 4000000</f>
@@ -2558,18 +2505,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B2" s="35">
         <v>10700000</v>
@@ -2581,7 +2528,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B3" s="35">
         <v>820000</v>
@@ -2611,15 +2558,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -2627,7 +2574,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B3">
         <v>1.4</v>
@@ -2635,7 +2582,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -2643,7 +2590,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -2651,7 +2598,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -2659,7 +2606,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -2667,7 +2614,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B8">
         <v>4</v>

</xml_diff>

<commit_message>
Excess info trimmed from info synthesis tab 3
</commit_message>
<xml_diff>
--- a/Excel Transcription of Data Analysis.xlsx
+++ b/Excel Transcription of Data Analysis.xlsx
@@ -540,15 +540,6 @@
     <t>- Built on site</t>
   </si>
   <si>
-    <t>- Roman arch (single/multiple); Segmental arch (single/multiple); Arch culvert (single/multiple)</t>
-  </si>
-  <si>
-    <t>- Beam type; Truss type</t>
-  </si>
-  <si>
-    <t>- Rigid, non-rigid; Three sided/Open footing/ Slab culvert, Four Sided; Arch topped, Rectangular</t>
-  </si>
-  <si>
     <t>- Assembled on site</t>
   </si>
   <si>
@@ -592,6 +583,15 @@
   </si>
   <si>
     <t xml:space="preserve">Usually have a high freeboard, therefore less vulnerable than other bridge types to increases in river level because of climate change. </t>
+  </si>
+  <si>
+    <t>Rigid, non-rigid; Three sided/Open footing/ Slab culvert, Four Sided; Arch topped, Rectangular</t>
+  </si>
+  <si>
+    <t>Beam type; Truss type</t>
+  </si>
+  <si>
+    <t>Roman arch (single/multiple); Segmental arch (single/multiple); Arch culvert (single/multiple)</t>
   </si>
 </sst>
 </file>
@@ -1208,10 +1208,10 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1308,22 +1308,22 @@
         <v>14</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>149</v>
@@ -1378,25 +1378,25 @@
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="J5" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="K5" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -1415,13 +1415,13 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="H6" s="10" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="I6" s="38" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1438,10 +1438,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>153</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>14</v>
@@ -1679,10 +1679,10 @@
         <v>14</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>82</v>

</xml_diff>